<commit_message>
Adjust Backlog to Reflect Needed activities for next sprint
</commit_message>
<xml_diff>
--- a/documentation/Product Backlog.xlsx
+++ b/documentation/Product Backlog.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jh00291\Documents\GitHub\SE2Project\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jn00041\Documents\GitHub\SE2Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EACB34F-DD02-444F-A09B-44B4CA9A1888}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CF5864-0D5A-44A0-B2D7-0209E3E3BE9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21540" yWindow="-26535" windowWidth="29400" windowHeight="22905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21540" yWindow="-26538" windowWidth="29400" windowHeight="22908" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -547,18 +548,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="153.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.41796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="153.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -572,7 +573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -586,7 +587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -600,7 +601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -614,7 +615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -628,7 +629,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -642,7 +643,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -656,7 +657,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -670,7 +671,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A9" s="6">
         <v>1</v>
       </c>
@@ -684,7 +685,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A10" s="6">
         <v>2</v>
       </c>
@@ -698,7 +699,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A11" s="6">
         <v>3</v>
       </c>
@@ -712,7 +713,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A12" s="6">
         <v>3</v>
       </c>
@@ -726,7 +727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A13" s="6">
         <v>3</v>
       </c>
@@ -740,7 +741,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A14" s="6">
         <v>3</v>
       </c>
@@ -754,7 +755,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A15">
         <v>4</v>
       </c>
@@ -768,7 +769,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A16">
         <v>4</v>
       </c>
@@ -782,7 +783,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="5">
         <v>5</v>
       </c>
@@ -796,7 +797,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="5">
         <v>5</v>
       </c>
@@ -810,7 +811,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A19" s="5">
         <v>6</v>
       </c>
@@ -824,7 +825,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A20" s="5">
         <v>6</v>
       </c>
@@ -838,7 +839,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A21" s="5">
         <v>6</v>
       </c>
@@ -852,7 +853,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A22" s="5">
         <v>6</v>
       </c>
@@ -866,7 +867,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A23">
         <v>6</v>
       </c>
@@ -880,7 +881,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A24">
         <v>6</v>
       </c>
@@ -894,7 +895,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>6</v>
       </c>
@@ -911,4 +912,16 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1407BF48-2D48-4D26-A282-EF11A05FEC2F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>